<commit_message>
Adding referral profile and modifying current profiles
</commit_message>
<xml_diff>
--- a/CodeSystem-SzEncounterClassificationCS.xlsx
+++ b/CodeSystem-SzEncounterClassificationCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-16T14:06:30+00:00</t>
+    <t>2025-08-01T12:25:19+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -120,7 +120,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>3</t>
+    <t>1</t>
   </si>
   <si>
     <t>Level</t>
@@ -135,25 +135,10 @@
     <t>Definition</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>OPD</t>
   </si>
   <si>
     <t>Out Patient Department</t>
-  </si>
-  <si>
-    <t>IPD</t>
-  </si>
-  <si>
-    <t>In Patient Department</t>
-  </si>
-  <si>
-    <t>EMG</t>
-  </si>
-  <si>
-    <t>Emergency</t>
   </si>
 </sst>
 </file>
@@ -464,7 +449,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -486,39 +471,15 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="C2" t="s" s="2">
-        <v>42</v>
-      </c>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>